<commit_message>
Fixes bug in proportions table
</commit_message>
<xml_diff>
--- a/Shiny/48-MIDAS_AMU/outputs/data_source_summary_table.xlsx
+++ b/Shiny/48-MIDAS_AMU/outputs/data_source_summary_table.xlsx
@@ -461,7 +461,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>22.87</t>
+          <t>45.74</t>
         </is>
       </c>
     </row>
@@ -473,7 +473,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>24.39</t>
+          <t>48.79</t>
         </is>
       </c>
     </row>
@@ -485,7 +485,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>0.16</t>
+          <t>0.32</t>
         </is>
       </c>
     </row>
@@ -497,7 +497,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>46.51</t>
+          <t>93.02</t>
         </is>
       </c>
     </row>
@@ -509,7 +509,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>3.47</t>
+          <t>6.94</t>
         </is>
       </c>
     </row>

</xml_diff>